<commit_message>
feat: Add all slug about B1
</commit_message>
<xml_diff>
--- a/src/data/b1.xlsx
+++ b/src/data/b1.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1A_xmumgithub\xmum-map\src\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F223A4-8B4A-4409-B73E-4C5B196CFE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="G" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="1" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="2" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="G" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="2" r:id="rId2"/>
+    <sheet name="2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -22,41 +27,83 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
-    <t xml:space="preserve">Name</t>
+    <t>Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Category</t>
+    <t>Category</t>
   </si>
   <si>
-    <t xml:space="preserve">Slug</t>
+    <t>Slug</t>
   </si>
   <si>
-    <t xml:space="preserve">Width</t>
+    <t>Width</t>
   </si>
   <si>
-    <t xml:space="preserve">Icon</t>
+    <t>Icon</t>
   </si>
   <si>
-    <t xml:space="preserve">Show</t>
+    <t>Show</t>
   </si>
   <si>
-    <t xml:space="preserve">Description</t>
+    <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Image</t>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Sapid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Restea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Astana Restaurant Sdn Bhd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poke Bowl Rice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zone U Bakery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>restaurant</t>
+  </si>
+  <si>
+    <t>snack</t>
+  </si>
+  <si>
+    <t>sapid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>restea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>astana</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>poke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bakery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -64,19 +111,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,138 +126,122 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18a303"/>
+        <a:srgbClr val="18A303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369a3"/>
+        <a:srgbClr val="0369A3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a33e03"/>
+        <a:srgbClr val="A33E03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8e03a3"/>
+        <a:srgbClr val="8E03A3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="c99c00"/>
+        <a:srgbClr val="C99C00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="c9211e"/>
+        <a:srgbClr val="C9211E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ee"/>
+        <a:srgbClr val="0000EE"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551a8b"/>
+        <a:srgbClr val="551A8B"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="DejaVu Sans"/>
+        <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -272,31 +294,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H86" activeCellId="0" sqref="H86"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="11.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="3" width="11.54"/>
+    <col min="1" max="2" width="11.54296875" style="1"/>
+    <col min="3" max="3" width="11.54296875" style="2"/>
+    <col min="4" max="6" width="11.54296875" style="1"/>
+    <col min="11" max="16384" width="11.54296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -322,616 +342,646 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+    <row r="2" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+    <row r="3" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+    <row r="4" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+    <row r="5" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+    <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
+    <row r="7" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
+    <row r="8" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
+    <row r="9" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
+    <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
+    <row r="11" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
+    <row r="12" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
+    <row r="13" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
+    <row r="14" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
+    <row r="15" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
+    <row r="16" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
+    <row r="17" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
+    <row r="18" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6"/>
+    <row r="19" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
+    <row r="20" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6"/>
+    <row r="21" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
+    <row r="22" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
+    <row r="23" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
+    <row r="24" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
+    <row r="25" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
+    <row r="26" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
+    <row r="27" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
+    <row r="28" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
+    <row r="29" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6"/>
+    <row r="30" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
+    <row r="31" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
+    <row r="32" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6"/>
+    <row r="33" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6"/>
+    <row r="34" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6"/>
+    <row r="35" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6"/>
+    <row r="36" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6"/>
+    <row r="37" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6"/>
+    <row r="38" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6"/>
+    <row r="39" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6"/>
+    <row r="40" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6"/>
+    <row r="41" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6"/>
+    <row r="42" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6"/>
+    <row r="43" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6"/>
+    <row r="44" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6"/>
+    <row r="45" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6"/>
+    <row r="46" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6"/>
+    <row r="47" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6"/>
+    <row r="48" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6"/>
+    <row r="49" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6"/>
+    <row r="50" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6"/>
+    <row r="51" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6"/>
+    <row r="52" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6"/>
+    <row r="53" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6"/>
+    <row r="54" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6"/>
+    <row r="55" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6"/>
+    <row r="56" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6"/>
+    <row r="57" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6"/>
+    <row r="58" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6"/>
+    <row r="59" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6"/>
+    <row r="60" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="6"/>
+    <row r="61" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="6"/>
+    <row r="62" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="6"/>
+    <row r="63" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="6"/>
+    <row r="64" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="6"/>
+    <row r="65" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="6"/>
+    <row r="66" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="6"/>
+    <row r="67" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="6"/>
+    <row r="68" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="6"/>
+    <row r="69" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6"/>
+    <row r="70" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6"/>
+    <row r="71" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="6"/>
+    <row r="72" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="6"/>
+    <row r="73" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="6"/>
+    <row r="74" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="7"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="6"/>
+    <row r="75" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="6"/>
+    <row r="76" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="7"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="6"/>
+    <row r="77" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="6"/>
+    <row r="78" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="7"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
@@ -939,16 +989,15 @@
       <c r="F78" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1 B79:B1001" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{858298F4-AE82-486E-9354-FE5E18C8576D}">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -956,24 +1005,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="3" width="11.54"/>
+    <col min="1" max="6" width="11.54296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -999,7 +1044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1007,7 +1052,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1015,7 +1060,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1023,7 +1068,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1031,7 +1076,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1039,7 +1084,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1047,7 +1092,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1055,7 +1100,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1063,7 +1108,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1071,7 +1116,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1079,7 +1124,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1087,7 +1132,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1095,7 +1140,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1103,7 +1148,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1111,7 +1156,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1119,7 +1164,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1127,7 +1172,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1135,7 +1180,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1143,7 +1188,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1151,7 +1196,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1159,7 +1204,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1167,7 +1212,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1175,7 +1220,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1183,7 +1228,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1191,7 +1236,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1199,7 +1244,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1207,7 +1252,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1215,7 +1260,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1223,7 +1268,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1231,7 +1276,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1239,7 +1284,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1247,7 +1292,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1255,7 +1300,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1263,7 +1308,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1271,7 +1316,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1279,7 +1324,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1287,7 +1332,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1295,7 +1340,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1303,7 +1348,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1311,7 +1356,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1319,7 +1364,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1327,7 +1372,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1335,7 +1380,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1343,7 +1388,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1351,7 +1396,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1359,7 +1404,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1367,7 +1412,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1375,7 +1420,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1383,7 +1428,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -1391,7 +1436,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -1399,7 +1444,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -1407,7 +1452,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -1415,7 +1460,7 @@
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1423,7 +1468,7 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -1431,7 +1476,7 @@
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -1439,7 +1484,7 @@
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1447,7 +1492,7 @@
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1455,7 +1500,7 @@
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -1463,7 +1508,7 @@
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -1471,7 +1516,7 @@
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -1479,7 +1524,7 @@
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -1487,7 +1532,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -1495,7 +1540,7 @@
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -1503,7 +1548,7 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -1511,7 +1556,7 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -1519,7 +1564,7 @@
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -1527,7 +1572,7 @@
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -1535,7 +1580,7 @@
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -1543,7 +1588,7 @@
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -1551,7 +1596,7 @@
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -1559,7 +1604,7 @@
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -1567,7 +1612,7 @@
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -1575,7 +1620,7 @@
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -1583,7 +1628,7 @@
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -1591,7 +1636,7 @@
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -1599,7 +1644,7 @@
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -1607,7 +1652,7 @@
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -1616,16 +1661,16 @@
       <c r="F78" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1 B79:B1001" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B79:B1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1633,24 +1678,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="3" width="11.54"/>
+    <col min="1" max="16384" width="11.54296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1676,281 +1717,281 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
-      <c r="E4" s="0"/>
-      <c r="F4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0"/>
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
-      <c r="F5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0"/>
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
-      <c r="E6" s="0"/>
-      <c r="F6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0"/>
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
-      <c r="F11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
-      <c r="F12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="D17" s="0"/>
-      <c r="E17" s="0"/>
-      <c r="F17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="D18" s="0"/>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-      <c r="E20" s="0"/>
-      <c r="F20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
-      <c r="E21" s="0"/>
-      <c r="F21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="B22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="D22" s="0"/>
-      <c r="E22" s="0"/>
-      <c r="F22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
-      <c r="E23" s="0"/>
-      <c r="F23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="0"/>
-      <c r="F24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
-      <c r="E25" s="0"/>
-      <c r="F25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
-      <c r="E26" s="0"/>
-      <c r="F26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="B27" s="0"/>
-      <c r="C27" s="0"/>
-      <c r="D27" s="0"/>
-      <c r="E27" s="0"/>
-      <c r="F27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
-      <c r="B28" s="0"/>
-      <c r="C28" s="0"/>
-      <c r="D28" s="0"/>
-      <c r="E28" s="0"/>
-      <c r="F28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-      <c r="B29" s="0"/>
-      <c r="C29" s="0"/>
-      <c r="D29" s="0"/>
-      <c r="E29" s="0"/>
-      <c r="F29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="0"/>
-      <c r="C30" s="0"/>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
-      <c r="B33" s="0"/>
-      <c r="C33" s="0"/>
-      <c r="D33" s="0"/>
-      <c r="E33" s="0"/>
-      <c r="F33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="B34" s="0"/>
-      <c r="C34" s="0"/>
-      <c r="D34" s="0"/>
-      <c r="E34" s="0"/>
-      <c r="F34" s="0"/>
+    <row r="2" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1 B35:B1001" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B35:B1001" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
chore: Generate the data.
</commit_message>
<xml_diff>
--- a/src/data/b1.xlsx
+++ b/src/data/b1.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1A_xmumgithub\xmum-map\src\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F223A4-8B4A-4409-B73E-4C5B196CFE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="G" sheetId="1" r:id="rId1"/>
-    <sheet name="1" sheetId="2" r:id="rId2"/>
-    <sheet name="2" sheetId="3" r:id="rId3"/>
+    <sheet name="G" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="1" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="2" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -29,81 +24,76 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Slug</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>Show</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>Sapid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Restea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Astana Restaurant Sdn Bhd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poke Bowl Rice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zone U Bakery</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>restaurant</t>
-  </si>
-  <si>
-    <t>snack</t>
-  </si>
-  <si>
-    <t>sapid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>restea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>astana</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>poke</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bakery</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sapid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restaurant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sapid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astana Restaurant Sdn Bhd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">astana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poke Bowl Rice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone U Bakery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bakery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -111,10 +101,19 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,122 +125,150 @@
     </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+  <cellXfs count="10">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="18A303"/>
+        <a:srgbClr val="18a303"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="0369A3"/>
+        <a:srgbClr val="0369a3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A33E03"/>
+        <a:srgbClr val="a33e03"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8E03A3"/>
+        <a:srgbClr val="8e03a3"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="C99C00"/>
+        <a:srgbClr val="c99c00"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="C9211E"/>
+        <a:srgbClr val="c9211e"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000EE"/>
+        <a:srgbClr val="0000ee"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="551A8B"/>
+        <a:srgbClr val="551a8b"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="DejaVu Sans"/>
-        <a:cs typeface="DejaVu Sans"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -294,29 +321,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="11.54296875" style="1"/>
-    <col min="3" max="3" width="11.54296875" style="2"/>
-    <col min="4" max="6" width="11.54296875" style="1"/>
-    <col min="11" max="16384" width="11.54296875" style="3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="3" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -342,77 +371,87 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -420,7 +459,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -428,7 +467,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -436,7 +475,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -444,7 +483,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -452,7 +491,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -460,7 +499,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -468,7 +507,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -476,7 +515,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -484,7 +523,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -492,7 +531,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -500,7 +539,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -508,7 +547,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -516,7 +555,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -524,7 +563,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -532,7 +571,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -540,7 +579,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -548,7 +587,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -556,7 +595,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -564,7 +603,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -572,7 +611,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -580,7 +619,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -588,7 +627,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -596,7 +635,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -604,7 +643,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -612,7 +651,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -620,7 +659,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="7"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -628,7 +667,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="7"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -636,7 +675,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -644,7 +683,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -652,7 +691,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -660,7 +699,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="7"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -668,7 +707,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="7"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -676,7 +715,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="7"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -684,7 +723,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -692,7 +731,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="7"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -700,7 +739,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="7"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -708,7 +747,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="7"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -716,7 +755,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="7"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -724,7 +763,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="7"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -732,7 +771,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="7"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -740,7 +779,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="7"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -748,7 +787,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="7"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -756,7 +795,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="7"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -764,7 +803,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="7"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -772,7 +811,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="7"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -780,7 +819,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="7"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -788,7 +827,7 @@
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -796,7 +835,7 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="7"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -804,7 +843,7 @@
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="7"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -812,7 +851,7 @@
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="7"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -820,7 +859,7 @@
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="7"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -828,7 +867,7 @@
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="7"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -836,7 +875,7 @@
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="7"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -844,7 +883,7 @@
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="7"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -852,7 +891,7 @@
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="7"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -860,7 +899,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="7"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -868,7 +907,7 @@
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="7"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -876,7 +915,7 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="7"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -884,7 +923,7 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="7"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -892,7 +931,7 @@
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="7"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -900,7 +939,7 @@
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="7"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -908,7 +947,7 @@
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="7"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -916,7 +955,7 @@
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="7"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -924,7 +963,7 @@
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="7"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -932,7 +971,7 @@
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="7"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -940,7 +979,7 @@
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="7"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -948,7 +987,7 @@
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="7"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -956,7 +995,7 @@
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="7"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -964,7 +1003,7 @@
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="7"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -972,7 +1011,7 @@
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="7"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -980,7 +1019,7 @@
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="7"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -989,15 +1028,16 @@
       <c r="F78" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{858298F4-AE82-486E-9354-FE5E18C8576D}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1:B1006" type="list">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1005,20 +1045,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="F2:F6 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="11.54296875" style="3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="3" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1052,7 +1096,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1060,7 +1104,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1068,7 +1112,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1076,7 +1120,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1084,7 +1128,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1092,7 +1136,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1100,7 +1144,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1108,7 +1152,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1116,7 +1160,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1124,7 +1168,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1132,7 +1176,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1140,7 +1184,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1148,7 +1192,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1156,7 +1200,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1164,7 +1208,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1172,7 +1216,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1180,7 +1224,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1188,7 +1232,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1196,7 +1240,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1204,7 +1248,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1212,7 +1256,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1220,7 +1264,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1228,7 +1272,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1236,7 +1280,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1244,7 +1288,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1252,7 +1296,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1260,7 +1304,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1268,7 +1312,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1276,7 +1320,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1284,7 +1328,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1292,7 +1336,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1300,7 +1344,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1308,7 +1352,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1316,7 +1360,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1324,7 +1368,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1332,7 +1376,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1340,7 +1384,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1348,7 +1392,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1356,7 +1400,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1364,7 +1408,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1372,7 +1416,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1380,7 +1424,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1388,7 +1432,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1396,7 +1440,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1404,7 +1448,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1412,7 +1456,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1420,7 +1464,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1428,7 +1472,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -1436,7 +1480,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -1444,7 +1488,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -1452,7 +1496,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -1460,7 +1504,7 @@
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1468,7 +1512,7 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -1476,7 +1520,7 @@
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -1484,7 +1528,7 @@
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1492,7 +1536,7 @@
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1500,7 +1544,7 @@
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -1508,7 +1552,7 @@
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -1516,7 +1560,7 @@
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -1524,7 +1568,7 @@
       <c r="E61" s="6"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -1532,7 +1576,7 @@
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -1540,7 +1584,7 @@
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -1548,7 +1592,7 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -1556,7 +1600,7 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -1564,7 +1608,7 @@
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -1572,7 +1616,7 @@
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -1580,7 +1624,7 @@
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -1588,7 +1632,7 @@
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -1596,7 +1640,7 @@
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -1604,7 +1648,7 @@
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -1612,7 +1656,7 @@
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -1620,7 +1664,7 @@
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -1628,7 +1672,7 @@
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -1636,7 +1680,7 @@
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -1644,7 +1688,7 @@
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -1652,7 +1696,7 @@
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -1661,16 +1705,16 @@
       <c r="F78" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B79:B1001" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1 B79:B1001" type="list">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1678,20 +1722,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="F2:F6 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="16384" width="11.54296875" style="3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="3" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1717,281 +1765,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-    </row>
+    <row r="2" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B35:B1001" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1 B35:B1001" type="list">
       <formula1>"restaurant,entertainment,snack,other,daily_necessity"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
feat: Add PLUXHealth Clinic.
</commit_message>
<xml_diff>
--- a/src/data/b1.xlsx
+++ b/src/data/b1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -80,6 +80,32 @@
   </si>
   <si>
     <t xml:space="preserve">bakery</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PLUXHealth Clinic
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="LXGW WenKai Mono"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">校内诊所</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">daily_necessity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1_clinic</t>
   </si>
 </sst>
 </file>
@@ -91,7 +117,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -112,6 +138,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="LXGW WenKai Mono"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,7 +194,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -202,6 +233,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -455,9 +490,15 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="A7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>

</xml_diff>